<commit_message>
bewerken + toevoegen playlist werkend
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3FE2C4-5906-4EA8-9FA5-477831300A39}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16463F4-454C-410D-B5A9-02166EDD34AE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,28 +127,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>

</xml_diff>

<commit_message>
add track + delete track werkend
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58205D62-842A-4682-AA76-C4FF044A9079}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7761D7-35B5-4598-BCDA-923FA6E53ED2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>Lees opdracht en check of je aan punten voldoet</t>
+  </si>
+  <si>
+    <t>WEEK 4</t>
+  </si>
+  <si>
+    <t>Add track to playlist</t>
+  </si>
+  <si>
+    <t>Remove track from playlist</t>
+  </si>
+  <si>
+    <t>Create package diagram</t>
+  </si>
+  <si>
+    <t>Create deployment diagram</t>
   </si>
 </sst>
 </file>
@@ -130,35 +145,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -194,8 +181,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46334063-8932-463E-BB77-51E4789AF441}" name="Tabel1" displayName="Tabel1" ref="C3:D26" totalsRowShown="0">
-  <autoFilter ref="C3:D26" xr:uid="{A2B2CB25-C1D8-46DE-A214-2B22DA0BBA50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46334063-8932-463E-BB77-51E4789AF441}" name="Tabel1" displayName="Tabel1" ref="C3:D35" totalsRowShown="0">
+  <autoFilter ref="C3:D35" xr:uid="{A2B2CB25-C1D8-46DE-A214-2B22DA0BBA50}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{190D0475-4C46-44F4-9130-A565565C76E4}" name="Task"/>
     <tableColumn id="2" xr3:uid="{105B33F4-7A62-422B-8CB7-7AE57BE69254}" name="Done"/>
@@ -467,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:D26"/>
+  <dimension ref="C3:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,15 +628,55 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D26">
+      <c r="D35">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:D30">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="C5:D25 C27:D30 D26">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>D5=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
connection close fix + random token fix
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7761D7-35B5-4598-BCDA-923FA6E53ED2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC00094-81FE-4DC1-B1B5-904446AC631B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Create deployment diagram</t>
+  </si>
+  <si>
+    <t>Token new generate when logout</t>
   </si>
 </sst>
 </file>
@@ -145,21 +148,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -456,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +655,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>22</v>
@@ -676,7 +673,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5:D25 C27:D30 D26">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>D5=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Identitmap tracks werkend + af
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7074A75B-DBBD-4FA0-8674-5B56210D6D6B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DE5751-52E6-40EE-A17D-CA22A9DA7D5F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -696,7 +696,7 @@
         <v>30</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>